<commit_message>
Navoiy va Toshkent shahar doklad oxirgi (bitta joy sariq qilinib qolib ketgan ekan)
</commit_message>
<xml_diff>
--- a/navoiy_indeks_2022_07.xlsx
+++ b/navoiy_indeks_2022_07.xlsx
@@ -5,21 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.ortiqov\Desktop\Cerr\Regular\Consumer confidence index\01_Survey_call_center\2022\02\consumer_sentiment\script\navoiy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.usmonov\Desktop\consumer_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645EAC80-8F49-48BE-BDC8-07BFDF42E5C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C36A00-D868-4692-9B15-AE31C7D44980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="13770" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="навоий_graph" sheetId="3" r:id="rId2"/>
     <sheet name="problems_district" sheetId="2" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1686,113 +1683,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="index"/>
-      <sheetName val="навоий_graph"/>
-      <sheetName val="problems_district"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="B1">
-            <v>44197</v>
-          </cell>
-          <cell r="C1">
-            <v>44287</v>
-          </cell>
-          <cell r="D1">
-            <v>44378</v>
-          </cell>
-          <cell r="E1">
-            <v>44470</v>
-          </cell>
-          <cell r="F1">
-            <v>44562</v>
-          </cell>
-          <cell r="G1">
-            <v>44652</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Кутилмалар индекси</v>
-          </cell>
-          <cell r="B2">
-            <v>165</v>
-          </cell>
-          <cell r="C2">
-            <v>162</v>
-          </cell>
-          <cell r="D2">
-            <v>145</v>
-          </cell>
-          <cell r="E2">
-            <v>152</v>
-          </cell>
-          <cell r="F2">
-            <v>164</v>
-          </cell>
-          <cell r="G2">
-            <v>158</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Умумий индекс</v>
-          </cell>
-          <cell r="B3">
-            <v>142</v>
-          </cell>
-          <cell r="C3">
-            <v>147</v>
-          </cell>
-          <cell r="D3">
-            <v>132</v>
-          </cell>
-          <cell r="E3">
-            <v>142</v>
-          </cell>
-          <cell r="F3">
-            <v>143</v>
-          </cell>
-          <cell r="G3">
-            <v>141</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Жорий ҳолат индекси</v>
-          </cell>
-          <cell r="B4">
-            <v>119</v>
-          </cell>
-          <cell r="C4">
-            <v>132</v>
-          </cell>
-          <cell r="D4">
-            <v>119</v>
-          </cell>
-          <cell r="E4">
-            <v>133</v>
-          </cell>
-          <cell r="F4">
-            <v>121</v>
-          </cell>
-          <cell r="G4">
-            <v>124</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2072,11 +1962,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2112,357 +2008,360 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="C2">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D2">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="E2">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F2">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="G2">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="H2">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="I2">
-        <v>125</v>
+        <v>153</v>
       </c>
       <c r="J2">
-        <v>145</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3">
+        <v>148</v>
+      </c>
+      <c r="C3">
         <v>134</v>
       </c>
-      <c r="C3">
-        <v>118</v>
-      </c>
       <c r="D3">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="E3">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F3">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="G3">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H3">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I3">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="J3">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C4">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="D4">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="E4">
         <v>133</v>
       </c>
       <c r="F4">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="G4">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="H4">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="I4">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="J4">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C5">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D5">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E5">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="F5">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G5">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="H5">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="I5">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="J5">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B6">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C6">
+        <v>121</v>
+      </c>
+      <c r="D6">
+        <v>167</v>
+      </c>
+      <c r="E6">
+        <v>124</v>
+      </c>
+      <c r="F6">
         <v>137</v>
       </c>
-      <c r="D6">
-        <v>149</v>
-      </c>
-      <c r="E6">
-        <v>120</v>
-      </c>
-      <c r="F6">
-        <v>135</v>
-      </c>
       <c r="G6">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H6">
-        <v>164</v>
+        <v>105</v>
       </c>
       <c r="I6">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="J6">
-        <v>166</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
+        <v>136</v>
+      </c>
+      <c r="C7">
+        <v>118</v>
+      </c>
+      <c r="D7">
+        <v>126</v>
+      </c>
+      <c r="E7">
+        <v>152</v>
+      </c>
+      <c r="F7">
+        <v>132</v>
+      </c>
+      <c r="G7">
+        <v>160</v>
+      </c>
+      <c r="H7">
+        <v>132</v>
+      </c>
+      <c r="I7">
         <v>128</v>
       </c>
-      <c r="C7">
-        <v>139</v>
-      </c>
-      <c r="D7">
-        <v>125</v>
-      </c>
-      <c r="E7">
-        <v>78</v>
-      </c>
-      <c r="F7">
-        <v>114</v>
-      </c>
-      <c r="G7">
-        <v>166</v>
-      </c>
-      <c r="H7">
-        <v>133</v>
-      </c>
-      <c r="I7">
-        <v>125</v>
-      </c>
       <c r="J7">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C8">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="D8">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="E8">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F8">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="G8">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H8">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="I8">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="J8">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C9">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D9">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="E9">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F9">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="G9">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="H9">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="I9">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="J9">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C10">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D10">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E10">
+        <v>116</v>
+      </c>
+      <c r="F10">
+        <v>112</v>
+      </c>
+      <c r="G10">
+        <v>162</v>
+      </c>
+      <c r="H10">
+        <v>147</v>
+      </c>
+      <c r="I10">
         <v>125</v>
       </c>
-      <c r="F10">
-        <v>121</v>
-      </c>
-      <c r="G10">
-        <v>159</v>
-      </c>
-      <c r="H10">
-        <v>125</v>
-      </c>
-      <c r="I10">
-        <v>133</v>
-      </c>
       <c r="J10">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11">
+        <v>128</v>
+      </c>
+      <c r="C11">
+        <v>139</v>
+      </c>
+      <c r="D11">
+        <v>125</v>
+      </c>
+      <c r="E11">
+        <v>78</v>
+      </c>
+      <c r="F11">
+        <v>114</v>
+      </c>
+      <c r="G11">
+        <v>166</v>
+      </c>
+      <c r="H11">
+        <v>133</v>
+      </c>
+      <c r="I11">
+        <v>125</v>
+      </c>
+      <c r="J11">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
         <v>138</v>
       </c>
-      <c r="C11">
-        <v>121</v>
-      </c>
-      <c r="D11">
-        <v>167</v>
-      </c>
-      <c r="E11">
-        <v>124</v>
-      </c>
-      <c r="F11">
-        <v>137</v>
-      </c>
-      <c r="G11">
-        <v>179</v>
-      </c>
-      <c r="H11">
-        <v>105</v>
-      </c>
-      <c r="I11">
-        <v>131</v>
-      </c>
-      <c r="J11">
+      <c r="C13">
+        <v>125</v>
+      </c>
+      <c r="D13">
+        <v>129</v>
+      </c>
+      <c r="E13">
+        <v>129</v>
+      </c>
+      <c r="F13">
+        <v>128</v>
+      </c>
+      <c r="G13">
+        <v>168</v>
+      </c>
+      <c r="H13">
+        <v>142</v>
+      </c>
+      <c r="I13">
         <v>138</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12">
-        <v>138</v>
-      </c>
-      <c r="C12">
-        <v>125</v>
-      </c>
-      <c r="D12">
-        <v>129</v>
-      </c>
-      <c r="E12">
-        <v>129</v>
-      </c>
-      <c r="F12">
-        <v>128</v>
-      </c>
-      <c r="G12">
-        <v>168</v>
-      </c>
-      <c r="H12">
-        <v>142</v>
-      </c>
-      <c r="I12">
-        <v>138</v>
-      </c>
-      <c r="J12">
+      <c r="J13">
         <v>149</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J11">
+    <sortCondition descending="1" ref="B2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -2472,7 +2371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82286774-0D3D-49BF-B80F-9B84F4EC8C62}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>